<commit_message>
fixed glm predict() for AG veg.
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{388A9C33-B354-4735-96EA-5487E7FEA33C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="6_{388A9C33-B354-4735-96EA-5487E7FEA33C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{536A23A1-7EA6-421A-BAB6-6958BEA1644B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="freq_table" sheetId="1" r:id="rId1"/>
     <sheet name="indicsp" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
   <si>
     <t>Species</t>
   </si>
@@ -143,22 +144,88 @@
     <t>Agrostis stolonifera*</t>
   </si>
   <si>
-    <t>Refrence</t>
-  </si>
-  <si>
-    <t>Above Ground Vegetation</t>
-  </si>
-  <si>
     <t>Below Ground Seed Bank</t>
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>Above Ground</t>
+  </si>
+  <si>
+    <t>Below Ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estuary </t>
+  </si>
+  <si>
+    <t>Time Since Disturbance</t>
+  </si>
+  <si>
+    <t>Disturbance condition</t>
+  </si>
+  <si>
+    <t>Revegetation status</t>
+  </si>
+  <si>
+    <t>Little Qualicum, Nanaimo</t>
+  </si>
+  <si>
+    <t>0 years (recent grubbing disturbance)</t>
+  </si>
+  <si>
+    <t>No transplants; ruderal vegetation exists</t>
+  </si>
+  <si>
+    <t>Nanaimo</t>
+  </si>
+  <si>
+    <t>1-year post-grazing/grubbing disturbance</t>
+  </si>
+  <si>
+    <t>Partially grubbed</t>
+  </si>
+  <si>
+    <t>No transplants; vegetation recovery from remnant and adjacent vegetation</t>
+  </si>
+  <si>
+    <t>Little Qualicum</t>
+  </si>
+  <si>
+    <t>10 years post-grazing/grubbing disturbance</t>
+  </si>
+  <si>
+    <t>No known grazing disturbance</t>
+  </si>
+  <si>
+    <t>No manipulations</t>
+  </si>
+  <si>
+    <t>Number of sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protected by exclosure? </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Number of surface seed bank samples per plot</t>
+  </si>
+  <si>
+    <t>Number of sampling plots per site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,8 +550,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -628,6 +701,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -673,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -704,19 +788,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1089,20 +1217,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="H1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="H1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -1764,23 +1892,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3114959-FF10-4595-A5F8-455218059366}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
     <col min="2" max="2" width="11.90625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="5"/>
-    <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="7.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12" style="21" customWidth="1"/>
+    <col min="8" max="8" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1801,8 +1931,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>41</v>
+      <c r="A2" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
@@ -1813,39 +1943,43 @@
       <c r="D2" s="10">
         <v>3.3E-3</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>34</v>
+      <c r="E2" s="18"/>
+      <c r="F2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="I2" s="10">
-        <v>1E-4</v>
+        <v>7.1999999999999998E-3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D3" s="10">
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="14" t="s">
+        <v>34</v>
+      </c>
       <c r="H3" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I3" s="10">
-        <v>4.58E-2</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="11" t="s">
         <v>34</v>
       </c>
@@ -1855,21 +1989,20 @@
       <c r="D4" s="10">
         <v>1E-4</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="11" t="s">
-        <v>1</v>
-      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I4" s="10">
-        <v>7.1999999999999998E-3</v>
+        <v>4.58E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -1877,9 +2010,10 @@
       <c r="D5" s="10">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>5</v>
@@ -1889,16 +2023,17 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="23">
         <v>2.4E-2</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="4" t="s">
         <v>38</v>
       </c>
@@ -1907,16 +2042,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="10">
         <v>3.95E-2</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1925,8 +2061,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1935,37 +2071,39 @@
       <c r="D8" s="10">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="23">
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="10">
         <v>2.64E-2</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="23">
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="B10" s="9" t="s">
         <v>36</v>
       </c>
@@ -1975,8 +2113,9 @@
       <c r="D10" s="10">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="9" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="22" t="s">
         <v>36</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -1986,17 +2125,285 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10">
+        <v>7.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="16"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10">
+        <v>4.58E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="16"/>
+      <c r="B15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1.5599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="10">
+        <v>3.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10">
+        <v>4.4900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="23">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="23">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G2:G3"/>
+  <mergeCells count="12">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="F2:F10"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="F2:F10"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF58E50-B3BE-49C4-B06D-2B4A5C7991F7}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.08984375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="7" max="7" width="9.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="24" customFormat="1" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="31">
+        <v>8</v>
+      </c>
+      <c r="G2" s="31">
+        <v>2</v>
+      </c>
+      <c r="H2" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="27">
+        <v>4</v>
+      </c>
+      <c r="G3" s="27">
+        <v>2</v>
+      </c>
+      <c r="H3" s="27">
+        <v>2</v>
+      </c>
+      <c r="P3" s="25"/>
+    </row>
+    <row r="4" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="29">
+        <v>4</v>
+      </c>
+      <c r="G4" s="29">
+        <v>2</v>
+      </c>
+      <c r="H4" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="29">
+        <v>8</v>
+      </c>
+      <c r="G5" s="29">
+        <v>2</v>
+      </c>
+      <c r="H5" s="29">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2232,18 +2639,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2266,26 +2673,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C387177-63B7-4B47-93D3-024ED4AF6CD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60909E04-0408-485E-AD28-829EC6C4040D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C387177-63B7-4B47-93D3-024ED4AF6CD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-    <ds:schemaRef ds:uri="8c008993-a31f-4b40-b1f3-88dd9c6e1924"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>